<commit_message>
Beta of direction control module
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joseph/Desktop/GitHub/Hardware-Modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F286CE9-654B-B048-BC7F-BFCC4BC64A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CC8CB6-28BE-3848-8C0C-8B0D60A4F996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{28D7BA6C-CDF7-D74F-9555-0B5674A136EB}"/>
+    <workbookView xWindow="17700" yWindow="0" windowWidth="11100" windowHeight="18000" activeTab="2" xr2:uid="{28D7BA6C-CDF7-D74F-9555-0B5674A136EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Code List" sheetId="2" r:id="rId1"/>
     <sheet name="Standard Module" sheetId="4" r:id="rId2"/>
-    <sheet name="Accessory Controller" sheetId="1" r:id="rId3"/>
+    <sheet name="Direction Controller" sheetId="5" r:id="rId3"/>
+    <sheet name="Accessory Controller" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="69">
   <si>
     <t>0x0C</t>
   </si>
@@ -87,6 +88,9 @@
     <t>0x06</t>
   </si>
   <si>
+    <t>0x07</t>
+  </si>
+  <si>
     <t>on(0x01) / off(0x02)</t>
   </si>
   <si>
@@ -163,6 +167,81 @@
   </si>
   <si>
     <t>Check Rear Buzzer</t>
+  </si>
+  <si>
+    <t>Disable Brake Motor Controller</t>
+  </si>
+  <si>
+    <t>Enable Brake Motor Controller</t>
+  </si>
+  <si>
+    <t>Disable Steering Motor Controller</t>
+  </si>
+  <si>
+    <t>Enable Steering Motor Controller</t>
+  </si>
+  <si>
+    <t>Reset Brake Motor Encoder Ticks</t>
+  </si>
+  <si>
+    <t>Is the brake motor enabled?</t>
+  </si>
+  <si>
+    <t>Get steering linear actuator potentiometer val</t>
+  </si>
+  <si>
+    <t>Is the steering motor enabled?</t>
+  </si>
+  <si>
+    <t>Get brake motor encoder ticks</t>
+  </si>
+  <si>
+    <t>{data}</t>
+  </si>
+  <si>
+    <t>Set brake motor position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set steering motor position </t>
+  </si>
+  <si>
+    <t>Set Steering Motor Power (Left)</t>
+  </si>
+  <si>
+    <t>Set Steering Motor Power (Right)</t>
+  </si>
+  <si>
+    <t>Set Brake Motor Power (Fwd)</t>
+  </si>
+  <si>
+    <t>Set Steering Motor Power (Rev)</t>
+  </si>
+  <si>
+    <t>Check Brake Pedal</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>Set wheel input (From wheel)</t>
+  </si>
+  <si>
+    <t>Set wheel input (From computer)</t>
+  </si>
+  <si>
+    <t>Set wheel turn speed (in manual mode)</t>
+  </si>
+  <si>
+    <t>Get current steering wheel potentiometer val</t>
+  </si>
+  <si>
+    <t>0x01 or 0x02</t>
+  </si>
+  <si>
+    <t>Is the steering mode manual?</t>
   </si>
 </sst>
 </file>
@@ -525,7 +604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF933041-708F-1D4E-A4AA-F0E0032867C3}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -599,7 +678,7 @@
   <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:O1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -614,7 +693,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
@@ -644,11 +723,11 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1">
         <v>0</v>
@@ -663,11 +742,822 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02849192-5AC6-354A-BD64-8500E72D5EC9}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="17" max="17" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="1">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>68</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>67</v>
+      </c>
+      <c r="R17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
+        <v>19</v>
+      </c>
+      <c r="T17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>53</v>
+      </c>
+      <c r="R18" t="s">
+        <v>53</v>
+      </c>
+      <c r="S18" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>50</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>53</v>
+      </c>
+      <c r="R19" t="s">
+        <v>53</v>
+      </c>
+      <c r="S19" t="s">
+        <v>19</v>
+      </c>
+      <c r="T19" t="s">
+        <v>19</v>
+      </c>
+      <c r="U19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>49</v>
+      </c>
+      <c r="N20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>67</v>
+      </c>
+      <c r="R20" t="s">
+        <v>19</v>
+      </c>
+      <c r="S20" t="s">
+        <v>19</v>
+      </c>
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>53</v>
+      </c>
+      <c r="R21" t="s">
+        <v>53</v>
+      </c>
+      <c r="S21" t="s">
+        <v>19</v>
+      </c>
+      <c r="T21" t="s">
+        <v>19</v>
+      </c>
+      <c r="U21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982E6C5A-A5E1-5E45-8E19-FDAC7DB57AC6}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -682,7 +1572,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
@@ -712,10 +1602,10 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N1" s="1">
         <v>0</v>
@@ -750,25 +1640,25 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -779,25 +1669,25 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -808,25 +1698,25 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -837,25 +1727,25 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -866,25 +1756,25 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -895,25 +1785,25 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -924,28 +1814,28 @@
         <v>11</v>
       </c>
       <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -956,28 +1846,28 @@
         <v>12</v>
       </c>
       <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -988,28 +1878,28 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -1020,28 +1910,28 @@
         <v>14</v>
       </c>
       <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -1052,28 +1942,28 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
         <v>31</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" t="s">
-        <v>29</v>
-      </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -1084,25 +1974,25 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N13" t="str">
         <f>B13</f>
@@ -1121,25 +2011,25 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N14" t="str">
         <f t="shared" ref="N14:O18" si="0">B14</f>
@@ -1158,25 +2048,25 @@
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N15" t="str">
         <f t="shared" si="0"/>
@@ -1195,25 +2085,25 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="N16" t="str">
         <f t="shared" si="0"/>
@@ -1232,25 +2122,25 @@
         <v>15</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N17" t="str">
         <f t="shared" si="0"/>
@@ -1269,25 +2159,25 @@
         <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N18" t="str">
         <f t="shared" si="0"/>
@@ -1296,6 +2186,35 @@
       <c r="O18" t="str">
         <f t="shared" si="0"/>
         <v>0x06</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beta of Modules (#7)
* Beta of direction control module

* Fix integer shifting

* Beta of accessory module

* CAN ID

* MCP4131 Lib

* MCP4131 Lib

* Fix comment

* Fix CAN interupt and periodic updates

* Store default CAN addresses

* Start speed controller

* Complete message list

* CAN message build utility

* Fix message

* Finish speed control module
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joseph/Desktop/GitHub/Hardware-Modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F286CE9-654B-B048-BC7F-BFCC4BC64A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A3C179-3586-F648-BE83-2EEC895352C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{28D7BA6C-CDF7-D74F-9555-0B5674A136EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Code List" sheetId="2" r:id="rId1"/>
-    <sheet name="Standard Module" sheetId="4" r:id="rId2"/>
-    <sheet name="Accessory Controller" sheetId="1" r:id="rId3"/>
+    <sheet name="STD Module" sheetId="7" r:id="rId2"/>
+    <sheet name="Speed Controller" sheetId="4" r:id="rId3"/>
+    <sheet name="Direction Controller" sheetId="5" r:id="rId4"/>
+    <sheet name="Accessory Controller" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="72">
   <si>
     <t>0x0C</t>
   </si>
@@ -87,6 +89,9 @@
     <t>0x06</t>
   </si>
   <si>
+    <t>0x07</t>
+  </si>
+  <si>
     <t>on(0x01) / off(0x02)</t>
   </si>
   <si>
@@ -111,18 +116,6 @@
     <t>Rear Buzzer (On/Off)</t>
   </si>
   <si>
-    <t>Blink Right Signal</t>
-  </si>
-  <si>
-    <t>Blink Left Signal</t>
-  </si>
-  <si>
-    <t>Blink Head Light</t>
-  </si>
-  <si>
-    <t>Blink Tail Light</t>
-  </si>
-  <si>
     <t>Honk Horn</t>
   </si>
   <si>
@@ -163,6 +156,102 @@
   </si>
   <si>
     <t>Check Rear Buzzer</t>
+  </si>
+  <si>
+    <t>Disable Brake Motor Controller</t>
+  </si>
+  <si>
+    <t>Enable Brake Motor Controller</t>
+  </si>
+  <si>
+    <t>Disable Steering Motor Controller</t>
+  </si>
+  <si>
+    <t>Enable Steering Motor Controller</t>
+  </si>
+  <si>
+    <t>Reset Brake Motor Encoder Ticks</t>
+  </si>
+  <si>
+    <t>Is the brake motor enabled?</t>
+  </si>
+  <si>
+    <t>Get steering linear actuator potentiometer val</t>
+  </si>
+  <si>
+    <t>Is the steering motor enabled?</t>
+  </si>
+  <si>
+    <t>Get brake motor encoder ticks</t>
+  </si>
+  <si>
+    <t>{data}</t>
+  </si>
+  <si>
+    <t>Set brake motor position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set steering motor position </t>
+  </si>
+  <si>
+    <t>Set Steering Motor Power (Left)</t>
+  </si>
+  <si>
+    <t>Set Steering Motor Power (Right)</t>
+  </si>
+  <si>
+    <t>Set Brake Motor Power (Fwd)</t>
+  </si>
+  <si>
+    <t>Set Steering Motor Power (Rev)</t>
+  </si>
+  <si>
+    <t>Check Brake Pedal</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x0E</t>
+  </si>
+  <si>
+    <t>Set wheel input (From wheel)</t>
+  </si>
+  <si>
+    <t>Set wheel input (From computer)</t>
+  </si>
+  <si>
+    <t>Set wheel turn speed (in manual mode)</t>
+  </si>
+  <si>
+    <t>Get current steering wheel potentiometer val</t>
+  </si>
+  <si>
+    <t>0x01 or 0x02</t>
+  </si>
+  <si>
+    <t>Is the steering mode manual?</t>
+  </si>
+  <si>
+    <t>Set default blinking interval</t>
+  </si>
+  <si>
+    <t>Set default horn interval</t>
+  </si>
+  <si>
+    <t>Set Direction to Forwards</t>
+  </si>
+  <si>
+    <t>Set Direction to Backwards</t>
+  </si>
+  <si>
+    <t>Get Direction</t>
+  </si>
+  <si>
+    <t>fwd 0x01, bkwd 0x02</t>
+  </si>
+  <si>
+    <t>Resp Code</t>
   </si>
 </sst>
 </file>
@@ -523,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF933041-708F-1D4E-A4AA-F0E0032867C3}">
-  <dimension ref="B2:D6"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +623,7 @@
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -544,8 +633,11 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>0</v>
       </c>
@@ -556,7 +648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>0</v>
       </c>
@@ -567,7 +659,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>0</v>
       </c>
@@ -577,8 +669,14 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>0</v>
       </c>
@@ -595,26 +693,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909B83E5-6C36-2547-ACA0-F96BFB726A97}">
-  <dimension ref="A1:O1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1744881B-86E2-F347-910B-7365FCFBBFA7}">
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A32" zoomScale="96" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="11" width="27.1640625" customWidth="1"/>
-    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
@@ -644,17 +742,35 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1">
         <v>0</v>
       </c>
       <c r="O1" s="1">
         <v>1</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -663,26 +779,1062 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982E6C5A-A5E1-5E45-8E19-FDAC7DB57AC6}">
-  <dimension ref="A1:U18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909B83E5-6C36-2547-ACA0-F96BFB726A97}">
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="16" max="16" width="20.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>57</v>
+      </c>
+      <c r="P17" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>19</v>
+      </c>
+      <c r="R17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
+        <v>19</v>
+      </c>
+      <c r="T17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02849192-5AC6-354A-BD64-8500E72D5EC9}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" customWidth="1"/>
+    <col min="10" max="10" width="41.83203125" customWidth="1"/>
+    <col min="11" max="11" width="27.1640625" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="17" max="17" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="1">
+        <v>0</v>
+      </c>
+      <c r="O1" s="1">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>3</v>
+      </c>
+      <c r="R1" s="1">
+        <v>4</v>
+      </c>
+      <c r="S1" s="1">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1">
+        <v>6</v>
+      </c>
+      <c r="U1" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>11</v>
+      </c>
+      <c r="P16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" t="s">
+        <v>64</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>11</v>
+      </c>
+      <c r="P17" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>63</v>
+      </c>
+      <c r="R17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
+        <v>19</v>
+      </c>
+      <c r="T17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>11</v>
+      </c>
+      <c r="P18" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>49</v>
+      </c>
+      <c r="R18" t="s">
+        <v>49</v>
+      </c>
+      <c r="S18" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>11</v>
+      </c>
+      <c r="P19" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>49</v>
+      </c>
+      <c r="R19" t="s">
+        <v>49</v>
+      </c>
+      <c r="S19" t="s">
+        <v>19</v>
+      </c>
+      <c r="T19" t="s">
+        <v>19</v>
+      </c>
+      <c r="U19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>45</v>
+      </c>
+      <c r="N20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>12</v>
+      </c>
+      <c r="P20" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>63</v>
+      </c>
+      <c r="R20" t="s">
+        <v>19</v>
+      </c>
+      <c r="S20" t="s">
+        <v>19</v>
+      </c>
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>48</v>
+      </c>
+      <c r="N21" t="s">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>12</v>
+      </c>
+      <c r="P21" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>49</v>
+      </c>
+      <c r="R21" t="s">
+        <v>49</v>
+      </c>
+      <c r="S21" t="s">
+        <v>19</v>
+      </c>
+      <c r="T21" t="s">
+        <v>19</v>
+      </c>
+      <c r="U21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{982E6C5A-A5E1-5E45-8E19-FDAC7DB57AC6}">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView zoomScale="81" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
-    <col min="10" max="10" width="41.83203125" customWidth="1"/>
-    <col min="11" max="11" width="27.1640625" customWidth="1"/>
-    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1">
         <v>0</v>
@@ -712,10 +1864,10 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N1" s="1">
         <v>0</v>
@@ -750,24 +1902,48 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
+        <v>19</v>
+      </c>
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -779,25 +1955,49 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="N3" t="s">
+        <v>19</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -808,25 +2008,49 @@
         <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -837,25 +2061,49 @@
         <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -866,25 +2114,49 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+      <c r="P6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" t="s">
+        <v>19</v>
+      </c>
+      <c r="T6" t="s">
+        <v>19</v>
+      </c>
+      <c r="U6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -895,25 +2167,49 @@
         <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="N7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O7" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>19</v>
+      </c>
+      <c r="R7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T7" t="s">
+        <v>19</v>
+      </c>
+      <c r="U7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -921,31 +2217,55 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" t="s">
-        <v>34</v>
+      <c r="N8" t="s">
+        <v>19</v>
+      </c>
+      <c r="O8" t="s">
+        <v>19</v>
+      </c>
+      <c r="P8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" t="s">
+        <v>19</v>
+      </c>
+      <c r="S8" t="s">
+        <v>19</v>
+      </c>
+      <c r="T8" t="s">
+        <v>19</v>
+      </c>
+      <c r="U8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
@@ -953,31 +2273,55 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" t="s">
-        <v>34</v>
+      <c r="N9" t="s">
+        <v>19</v>
+      </c>
+      <c r="O9" t="s">
+        <v>19</v>
+      </c>
+      <c r="P9" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" t="s">
+        <v>19</v>
+      </c>
+      <c r="S9" t="s">
+        <v>19</v>
+      </c>
+      <c r="T9" t="s">
+        <v>19</v>
+      </c>
+      <c r="U9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
@@ -985,31 +2329,55 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" t="s">
-        <v>34</v>
+      <c r="N10" t="s">
+        <v>19</v>
+      </c>
+      <c r="O10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S10" t="s">
+        <v>19</v>
+      </c>
+      <c r="T10" t="s">
+        <v>19</v>
+      </c>
+      <c r="U10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -1017,31 +2385,55 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
         <v>31</v>
       </c>
-      <c r="E11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" t="s">
-        <v>28</v>
-      </c>
-      <c r="K11" t="s">
-        <v>34</v>
+      <c r="N11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O11" t="s">
+        <v>19</v>
+      </c>
+      <c r="P11" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" t="s">
+        <v>19</v>
+      </c>
+      <c r="S11" t="s">
+        <v>19</v>
+      </c>
+      <c r="T11" t="s">
+        <v>19</v>
+      </c>
+      <c r="U11" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
@@ -1049,31 +2441,55 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" t="s">
-        <v>33</v>
+      <c r="N12" t="s">
+        <v>19</v>
+      </c>
+      <c r="O12" t="s">
+        <v>19</v>
+      </c>
+      <c r="P12" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>19</v>
+      </c>
+      <c r="R12" t="s">
+        <v>19</v>
+      </c>
+      <c r="S12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
@@ -1081,36 +2497,52 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
-      </c>
-      <c r="N13" t="str">
-        <f>B13</f>
-        <v>0x0C</v>
-      </c>
-      <c r="O13" t="str">
-        <f>C13</f>
-        <v>0x01</v>
+        <v>34</v>
+      </c>
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>4</v>
+      </c>
+      <c r="P13" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" t="s">
+        <v>19</v>
+      </c>
+      <c r="T13" t="s">
+        <v>19</v>
+      </c>
+      <c r="U13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
@@ -1118,36 +2550,52 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
-      </c>
-      <c r="N14" t="str">
-        <f t="shared" ref="N14:O18" si="0">B14</f>
-        <v>0x0C</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="0"/>
-        <v>0x02</v>
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P14" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>63</v>
+      </c>
+      <c r="R14" t="s">
+        <v>19</v>
+      </c>
+      <c r="S14" t="s">
+        <v>19</v>
+      </c>
+      <c r="T14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
@@ -1155,36 +2603,52 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
-      </c>
-      <c r="N15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x0C</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="0"/>
-        <v>0x03</v>
+        <v>36</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>4</v>
+      </c>
+      <c r="P15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>63</v>
+      </c>
+      <c r="R15" t="s">
+        <v>19</v>
+      </c>
+      <c r="S15" t="s">
+        <v>19</v>
+      </c>
+      <c r="T15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
@@ -1192,110 +2656,317 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
       <c r="E16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
-        <v>40</v>
-      </c>
-      <c r="N16" t="str">
-        <f t="shared" si="0"/>
-        <v>0x0C</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="0"/>
-        <v>0x04</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>4</v>
+      </c>
+      <c r="P16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>0</v>
       </c>
       <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
       <c r="E17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
-        <v>41</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="0"/>
-        <v>0x0C</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="0"/>
-        <v>0x05</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>63</v>
+      </c>
+      <c r="R17" t="s">
+        <v>19</v>
+      </c>
+      <c r="S17" t="s">
+        <v>19</v>
+      </c>
+      <c r="T17" t="s">
+        <v>19</v>
+      </c>
+      <c r="U17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>0</v>
       </c>
       <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
-        <v>42</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="0"/>
-        <v>0x0C</v>
-      </c>
-      <c r="O18" t="str">
-        <f t="shared" si="0"/>
-        <v>0x06</v>
+        <v>39</v>
+      </c>
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>63</v>
+      </c>
+      <c r="R18" t="s">
+        <v>19</v>
+      </c>
+      <c r="S18" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" t="s">
+        <v>19</v>
+      </c>
+      <c r="U18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+      <c r="J19" t="s">
+        <v>56</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>63</v>
+      </c>
+      <c r="R19" t="s">
+        <v>19</v>
+      </c>
+      <c r="S19" t="s">
+        <v>19</v>
+      </c>
+      <c r="T19" t="s">
+        <v>19</v>
+      </c>
+      <c r="U19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" t="s">
+        <v>65</v>
+      </c>
+      <c r="N20" t="s">
+        <v>19</v>
+      </c>
+      <c r="O20" t="s">
+        <v>19</v>
+      </c>
+      <c r="P20" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>19</v>
+      </c>
+      <c r="R20" t="s">
+        <v>19</v>
+      </c>
+      <c r="S20" t="s">
+        <v>19</v>
+      </c>
+      <c r="T20" t="s">
+        <v>19</v>
+      </c>
+      <c r="U20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" t="s">
+        <v>19</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" t="s">
+        <v>66</v>
+      </c>
+      <c r="N21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O21" t="s">
+        <v>19</v>
+      </c>
+      <c r="P21" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>19</v>
+      </c>
+      <c r="R21" t="s">
+        <v>19</v>
+      </c>
+      <c r="S21" t="s">
+        <v>19</v>
+      </c>
+      <c r="T21" t="s">
+        <v>19</v>
+      </c>
+      <c r="U21" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish Message List (#8)
* Finish Message List
</commit_message>
<xml_diff>
--- a/Protocol.xlsx
+++ b/Protocol.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Joseph/Desktop/GitHub/Hardware-Modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A3C179-3586-F648-BE83-2EEC895352C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2395565-3FA9-124E-88F9-E238672AF371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{28D7BA6C-CDF7-D74F-9555-0B5674A136EB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="88">
   <si>
     <t>0x0C</t>
   </si>
@@ -252,6 +252,54 @@
   </si>
   <si>
     <t>Resp Code</t>
+  </si>
+  <si>
+    <t>Enable Automatic Reverse Buzzer</t>
+  </si>
+  <si>
+    <t>Disable Automatic Reverse Buzzer</t>
+  </si>
+  <si>
+    <t>Get Buzzer Status</t>
+  </si>
+  <si>
+    <t>en 0x01, dis 0x02</t>
+  </si>
+  <si>
+    <t>Enable Accelerator</t>
+  </si>
+  <si>
+    <t>Disable Accelerator</t>
+  </si>
+  <si>
+    <t>Set Accelerator to Manual Input</t>
+  </si>
+  <si>
+    <t>Set Accelerator to Digital Input</t>
+  </si>
+  <si>
+    <t>Set Digital Acclerator Wiper Pos</t>
+  </si>
+  <si>
+    <t>Increment Digital Accelerator Wiper</t>
+  </si>
+  <si>
+    <t>Decrement Digital Accelerator Wiper</t>
+  </si>
+  <si>
+    <t>Get Accelerator Wiper Pos</t>
+  </si>
+  <si>
+    <t>Get Accelerator Input Selection</t>
+  </si>
+  <si>
+    <t>Is Accelerator Enabled</t>
+  </si>
+  <si>
+    <t>man 0x01, dig 0x02</t>
+  </si>
+  <si>
+    <t>{data]</t>
   </si>
 </sst>
 </file>
@@ -615,7 +663,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -782,8 +830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909B83E5-6C36-2547-ACA0-F96BFB726A97}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M75" sqref="M75"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -793,7 +841,9 @@
     <col min="10" max="10" width="41.83203125" customWidth="1"/>
     <col min="11" max="11" width="27.1640625" customWidth="1"/>
     <col min="13" max="13" width="8.5" customWidth="1"/>
-    <col min="16" max="16" width="20.5" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -859,9 +909,154 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
         <v>57</v>
@@ -890,7 +1085,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>57</v>
@@ -919,7 +1114,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
         <v>57</v>
@@ -942,6 +1137,308 @@
       <c r="I9" t="s">
         <v>19</v>
       </c>
+      <c r="J9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" t="s">
+        <v>83</v>
+      </c>
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>4</v>
+      </c>
+      <c r="R13" t="s">
+        <v>87</v>
+      </c>
+      <c r="S13" t="s">
+        <v>19</v>
+      </c>
+      <c r="T13" t="s">
+        <v>19</v>
+      </c>
+      <c r="U13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" t="s">
+        <v>84</v>
+      </c>
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>57</v>
+      </c>
+      <c r="R14" t="s">
+        <v>75</v>
+      </c>
+      <c r="S14" t="s">
+        <v>19</v>
+      </c>
+      <c r="T14" t="s">
+        <v>19</v>
+      </c>
+      <c r="U14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>58</v>
+      </c>
+      <c r="R15" t="s">
+        <v>86</v>
+      </c>
+      <c r="S15" t="s">
+        <v>19</v>
+      </c>
+      <c r="T15" t="s">
+        <v>19</v>
+      </c>
+      <c r="U15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>74</v>
+      </c>
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>75</v>
+      </c>
+      <c r="R16" t="s">
+        <v>19</v>
+      </c>
+      <c r="S16" t="s">
+        <v>19</v>
+      </c>
+      <c r="T16" t="s">
+        <v>19</v>
+      </c>
+      <c r="U16" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
@@ -975,13 +1472,13 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
         <v>57</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>70</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>19</v>
       </c>
       <c r="R17" t="s">
         <v>19</v>
@@ -1006,8 +1503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02849192-5AC6-354A-BD64-8500E72D5EC9}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="B1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1521,16 +2018,16 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
         <v>11</v>
       </c>
-      <c r="P16" t="s">
-        <v>4</v>
-      </c>
       <c r="Q16" t="s">
+        <v>4</v>
+      </c>
+      <c r="R16" t="s">
         <v>63</v>
-      </c>
-      <c r="R16" t="s">
-        <v>19</v>
       </c>
       <c r="S16" t="s">
         <v>19</v>
@@ -1574,16 +2071,16 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
         <v>11</v>
       </c>
-      <c r="P17" t="s">
+      <c r="Q17" t="s">
         <v>57</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>63</v>
-      </c>
-      <c r="R17" t="s">
-        <v>19</v>
       </c>
       <c r="S17" t="s">
         <v>19</v>
@@ -1627,19 +2124,19 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
         <v>11</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" t="s">
         <v>58</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>49</v>
       </c>
       <c r="R18" t="s">
         <v>49</v>
       </c>
       <c r="S18" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -1680,19 +2177,19 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
         <v>11</v>
       </c>
-      <c r="P19" t="s">
+      <c r="Q19" t="s">
         <v>7</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>49</v>
       </c>
       <c r="R19" t="s">
         <v>49</v>
       </c>
       <c r="S19" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -1733,16 +2230,16 @@
         <v>0</v>
       </c>
       <c r="O20" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
         <v>12</v>
       </c>
-      <c r="P20" t="s">
-        <v>4</v>
-      </c>
       <c r="Q20" t="s">
+        <v>4</v>
+      </c>
+      <c r="R20" t="s">
         <v>63</v>
-      </c>
-      <c r="R20" t="s">
-        <v>19</v>
       </c>
       <c r="S20" t="s">
         <v>19</v>
@@ -1786,19 +2283,19 @@
         <v>0</v>
       </c>
       <c r="O21" t="s">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
         <v>12</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" t="s">
         <v>7</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>49</v>
       </c>
       <c r="R21" t="s">
         <v>49</v>
       </c>
       <c r="S21" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -1818,7 +2315,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView zoomScale="81" workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2524,16 +3021,16 @@
         <v>0</v>
       </c>
       <c r="O13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P13" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q13" t="s">
         <v>11</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>63</v>
-      </c>
-      <c r="R13" t="s">
-        <v>19</v>
       </c>
       <c r="S13" t="s">
         <v>19</v>
@@ -2577,16 +3074,16 @@
         <v>0</v>
       </c>
       <c r="O14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P14" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q14" t="s">
         <v>12</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>63</v>
-      </c>
-      <c r="R14" t="s">
-        <v>19</v>
       </c>
       <c r="S14" t="s">
         <v>19</v>
@@ -2630,16 +3127,16 @@
         <v>0</v>
       </c>
       <c r="O15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P15" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q15" t="s">
         <v>13</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>63</v>
-      </c>
-      <c r="R15" t="s">
-        <v>19</v>
       </c>
       <c r="S15" t="s">
         <v>19</v>
@@ -2683,16 +3180,16 @@
         <v>0</v>
       </c>
       <c r="O16" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>63</v>
-      </c>
-      <c r="R16" t="s">
-        <v>19</v>
       </c>
       <c r="S16" t="s">
         <v>19</v>
@@ -2736,16 +3233,16 @@
         <v>0</v>
       </c>
       <c r="O17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P17" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q17" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>63</v>
-      </c>
-      <c r="R17" t="s">
-        <v>19</v>
       </c>
       <c r="S17" t="s">
         <v>19</v>
@@ -2789,16 +3286,16 @@
         <v>0</v>
       </c>
       <c r="O18" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P18" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>63</v>
-      </c>
-      <c r="R18" t="s">
-        <v>19</v>
       </c>
       <c r="S18" t="s">
         <v>19</v>
@@ -2842,16 +3339,16 @@
         <v>0</v>
       </c>
       <c r="O19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="P19" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q19" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>63</v>
-      </c>
-      <c r="R19" t="s">
-        <v>19</v>
       </c>
       <c r="S19" t="s">
         <v>19</v>

</xml_diff>